<commit_message>
Corrected Movie_DB for fake names
</commit_message>
<xml_diff>
--- a/Movie_clustering/Movie_DB.xlsx
+++ b/Movie_clustering/Movie_DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriangoik/Desktop/NAI_toolsAI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriangoik/PycharmProjects/PersonalProjectsAI/Movie_clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6D36BA6-7FC8-1E43-BF72-9E3A51F9A470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2776204-C669-4941-8C19-4E7619FFC6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16300" xr2:uid="{14215497-3E52-6B4A-80E9-8F4D9FD0AEAD}"/>
+    <workbookView xWindow="280" yWindow="760" windowWidth="28240" windowHeight="16300" xr2:uid="{14215497-3E52-6B4A-80E9-8F4D9FD0AEAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Oceny (1 słaby - 10 doskonały)</t>
   </si>
   <si>
-    <t>Paweł Czapiewski</t>
-  </si>
-  <si>
     <t>Jak sprzedawać dragi w sieci (szybko)</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>La Cara Oculta</t>
   </si>
   <si>
-    <t>Łukasz Bosak</t>
-  </si>
-  <si>
     <t>Star wars nowa trylogia</t>
   </si>
   <si>
@@ -268,9 +262,6 @@
     <t>Cube</t>
   </si>
   <si>
-    <t>Mariusz Buhaj</t>
-  </si>
-  <si>
     <t>Jak sprzedawać</t>
   </si>
   <si>
@@ -355,9 +346,6 @@
     <t>Strażnicy galaktyki</t>
   </si>
   <si>
-    <t>Aleksander Opałka</t>
-  </si>
-  <si>
     <t>Mr.Robot</t>
   </si>
   <si>
@@ -433,9 +421,6 @@
     <t>Rick i Morty</t>
   </si>
   <si>
-    <t>Szymon Rosztajn</t>
-  </si>
-  <si>
     <t>Star Wars III</t>
   </si>
   <si>
@@ -511,9 +496,6 @@
     <t>Auta 3</t>
   </si>
   <si>
-    <t>Mateusz Lech</t>
-  </si>
-  <si>
     <t>W tłumie</t>
   </si>
   <si>
@@ -706,9 +688,6 @@
     <t>Iron man 3</t>
   </si>
   <si>
-    <t>Łukasz Soldatke</t>
-  </si>
-  <si>
     <t>Bravehearth</t>
   </si>
   <si>
@@ -739,9 +718,6 @@
     <t>Rocky 1-5</t>
   </si>
   <si>
-    <t>Artur Szulc</t>
-  </si>
-  <si>
     <t>Dead Pool &amp; wolverine</t>
   </si>
   <si>
@@ -808,9 +784,6 @@
     <t>Gdzie jest Nemo?</t>
   </si>
   <si>
-    <t>Marta Szpilka</t>
-  </si>
-  <si>
     <t>Lobster</t>
   </si>
   <si>
@@ -896,6 +869,33 @@
   </si>
   <si>
     <t>Blow</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Łukasz Kowalski</t>
+  </si>
+  <si>
+    <t>Maricin Iksiński</t>
+  </si>
+  <si>
+    <t>Karol Kowal</t>
+  </si>
+  <si>
+    <t>Szymon Czerwiński</t>
+  </si>
+  <si>
+    <t>Lech Matczak</t>
+  </si>
+  <si>
+    <t>Paulina Włodarczyk</t>
+  </si>
+  <si>
+    <t>Ian Smith</t>
+  </si>
+  <si>
+    <t>Dawid Lancer</t>
   </si>
 </sst>
 </file>
@@ -992,9 +992,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1032,7 +1032,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1138,7 +1138,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1280,7 +1280,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1291,10 +1291,13 @@
   <dimension ref="A1:CE12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:83">
       <c r="A1" s="1" t="s">
@@ -1385,7 +1388,7 @@
     </row>
     <row r="2" spans="1:83">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>278</v>
       </c>
       <c r="B2" s="3">
         <v>1670</v>
@@ -1394,49 +1397,49 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2">
+        <v>9</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="I2" s="2">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="K2" s="2">
         <v>3</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3">
+        <v>9</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="3">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="O2" s="2">
         <v>7</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="3">
         <v>8</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S2" s="2">
         <v>10</v>
@@ -1448,187 +1451,187 @@
         <v>10</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W2" s="2">
         <v>8</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>9</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="AE2" s="2">
         <v>5</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG2" s="2">
         <v>6</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AI2" s="2">
         <v>3</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AK2" s="2">
         <v>2</v>
       </c>
       <c r="AL2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>9</v>
+      </c>
+      <c r="AN2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AM2" s="2">
-        <v>9</v>
-      </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2">
+        <v>7</v>
+      </c>
+      <c r="AR2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="AS2" s="2">
         <v>2</v>
       </c>
       <c r="AT2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>10</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AU2" s="2">
-        <v>10</v>
-      </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="2">
+        <v>10</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AW2" s="2">
-        <v>10</v>
-      </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="2">
+        <v>9</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="AY2" s="2">
-        <v>9</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="BA2" s="2">
         <v>1</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BC2" s="2">
         <v>1</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="BE2" s="2">
         <v>2</v>
       </c>
       <c r="BF2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>9</v>
+      </c>
+      <c r="BH2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="BG2" s="2">
-        <v>9</v>
-      </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BI2" s="2">
+        <v>9</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="BI2" s="2">
-        <v>9</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="BK2" s="2">
         <v>1</v>
       </c>
       <c r="BL2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="BM2" s="2">
+        <v>7</v>
+      </c>
+      <c r="BN2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="BM2" s="2">
-        <v>7</v>
-      </c>
-      <c r="BN2" s="2" t="s">
+      <c r="BO2" s="2">
+        <v>10</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="BO2" s="2">
-        <v>10</v>
-      </c>
-      <c r="BP2" s="2" t="s">
+      <c r="BQ2" s="2">
+        <v>8</v>
+      </c>
+      <c r="BR2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="BQ2" s="2">
-        <v>8</v>
-      </c>
-      <c r="BR2" s="2" t="s">
+      <c r="BS2" s="2">
+        <v>8</v>
+      </c>
+      <c r="BT2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="BS2" s="2">
-        <v>8</v>
-      </c>
-      <c r="BT2" s="2" t="s">
+      <c r="BU2" s="2">
+        <v>10</v>
+      </c>
+      <c r="BV2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BU2" s="2">
-        <v>10</v>
-      </c>
-      <c r="BV2" s="2" t="s">
+      <c r="BW2" s="2">
+        <v>9</v>
+      </c>
+      <c r="BX2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="BW2" s="2">
-        <v>9</v>
-      </c>
-      <c r="BX2" s="2" t="s">
+      <c r="BY2" s="2">
+        <v>8</v>
+      </c>
+      <c r="BZ2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="BY2" s="2">
-        <v>8</v>
-      </c>
-      <c r="BZ2" s="2" t="s">
+      <c r="CA2" s="2">
+        <v>9</v>
+      </c>
+      <c r="CB2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="CA2" s="2">
-        <v>9</v>
-      </c>
-      <c r="CB2" s="2" t="s">
+      <c r="CC2" s="2">
+        <v>9</v>
+      </c>
+      <c r="CD2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="CC2" s="2">
-        <v>9</v>
-      </c>
-      <c r="CD2" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="CE2" s="2">
         <v>10</v>
@@ -1636,7 +1639,7 @@
     </row>
     <row r="3" spans="1:83">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="B3" s="2">
         <v>1670</v>
@@ -1645,241 +1648,241 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="2">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="2">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2">
+        <v>9</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="I3" s="2">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="2">
-        <v>9</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O3" s="2">
         <v>8</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="2">
         <v>8</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S3" s="2">
         <v>3</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="2">
+        <v>9</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="2">
+        <v>9</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="U3" s="2">
-        <v>9</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="2">
-        <v>9</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y3" s="2">
-        <v>7</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="AA3" s="2">
         <v>1</v>
       </c>
       <c r="AB3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>7</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" s="2">
-        <v>7</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AG3" s="2">
+        <v>9</v>
+      </c>
+      <c r="AH3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AE3" s="2">
-        <v>7</v>
-      </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AI3" s="2">
+        <v>10</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>9</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>10</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="AK3" s="2">
         <v>2</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AM3" s="2">
         <v>8</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AO3" s="2">
         <v>5</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AQ3" s="2">
         <v>7</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS3" s="2">
         <v>3</v>
       </c>
       <c r="AT3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>9</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW3" s="2">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="AU3" s="2">
-        <v>9</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AW3" s="2">
-        <v>10</v>
-      </c>
-      <c r="AX3" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="AY3" s="2">
         <v>1</v>
       </c>
       <c r="AZ3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="BA3" s="2">
         <v>9</v>
       </c>
       <c r="BB3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BC3" s="2">
         <v>6</v>
       </c>
       <c r="BD3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="BE3" s="2">
         <v>3</v>
       </c>
       <c r="BF3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BG3" s="2">
+        <v>8</v>
+      </c>
+      <c r="BH3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BK3" s="2">
+        <v>10</v>
+      </c>
+      <c r="BL3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="BG3" s="2">
-        <v>8</v>
-      </c>
-      <c r="BH3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="BI3" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
+      <c r="BM3" s="2">
+        <v>7</v>
+      </c>
+      <c r="BN3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="BK3" s="2">
-        <v>10</v>
-      </c>
-      <c r="BL3" s="2" t="s">
+      <c r="BO3" s="2">
+        <v>9</v>
+      </c>
+      <c r="BP3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="BM3" s="2">
-        <v>7</v>
-      </c>
-      <c r="BN3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BO3" s="2">
-        <v>9</v>
-      </c>
-      <c r="BP3" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="BQ3" s="2">
         <v>6</v>
       </c>
       <c r="BR3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BS3" s="2">
         <v>5</v>
       </c>
       <c r="BT3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BU3" s="2">
         <v>9</v>
       </c>
       <c r="BV3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW3" s="2">
+        <v>7</v>
+      </c>
+      <c r="BX3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY3" s="2">
+        <v>7</v>
+      </c>
+      <c r="BZ3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="CA3" s="2">
+        <v>8</v>
+      </c>
+      <c r="CB3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BW3" s="2">
-        <v>7</v>
-      </c>
-      <c r="BX3" s="2" t="s">
+      <c r="CC3" s="2">
+        <v>7</v>
+      </c>
+      <c r="CD3" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="BY3" s="2">
-        <v>7</v>
-      </c>
-      <c r="BZ3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="CA3" s="2">
-        <v>8</v>
-      </c>
-      <c r="CB3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="CC3" s="2">
-        <v>7</v>
-      </c>
-      <c r="CD3" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="CE3" s="2">
         <v>4</v>
@@ -1887,7 +1890,7 @@
     </row>
     <row r="4" spans="1:83">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>280</v>
       </c>
       <c r="B4" s="3">
         <v>1670</v>
@@ -1896,241 +1899,241 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="2">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="2">
+        <v>8</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="2">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="M4" s="2">
+        <v>9</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="2">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="O4" s="2">
+        <v>7</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="2">
-        <v>8</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="Q4" s="2">
+        <v>8</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="M4" s="2">
-        <v>9</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O4" s="2">
-        <v>7</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>8</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="S4" s="2">
         <v>1</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="U4" s="2">
         <v>9</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W4" s="2">
         <v>3</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="2">
         <v>6</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA4" s="2">
         <v>4</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AC4" s="2">
         <v>1</v>
       </c>
       <c r="AD4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>10</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AE4" s="2">
-        <v>8</v>
-      </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AM4" s="2">
+        <v>8</v>
+      </c>
+      <c r="AN4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AG4" s="2">
-        <v>10</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AI4" s="2">
-        <v>8</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK4" s="2">
-        <v>8</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM4" s="2">
-        <v>8</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="AO4" s="2">
         <v>7</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AQ4" s="2">
         <v>2</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AS4" s="2">
         <v>3</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AU4" s="2">
         <v>7</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AW4" s="2">
         <v>6</v>
       </c>
       <c r="AX4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AY4" s="2">
         <v>2</v>
       </c>
       <c r="AZ4" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="BA4" s="2">
         <v>9</v>
       </c>
       <c r="BB4" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="BC4" s="2">
         <v>6</v>
       </c>
       <c r="BD4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BE4" s="2">
         <v>8</v>
       </c>
       <c r="BF4" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="BG4" s="2">
         <v>10</v>
       </c>
       <c r="BH4" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="BI4" s="2">
         <v>9</v>
       </c>
       <c r="BJ4" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="BK4" s="2">
         <v>3</v>
       </c>
       <c r="BL4" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="BM4" s="2">
         <v>2</v>
       </c>
       <c r="BN4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BO4" s="2">
         <v>4</v>
       </c>
       <c r="BP4" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="BQ4" s="2">
         <v>3</v>
       </c>
       <c r="BR4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="BS4" s="2">
         <v>5</v>
       </c>
       <c r="BT4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="BU4" s="2">
         <v>5</v>
       </c>
       <c r="BV4" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="BW4" s="2">
         <v>6</v>
       </c>
       <c r="BX4" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="BY4" s="2">
         <v>4</v>
       </c>
       <c r="BZ4" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="CA4" s="2">
         <v>4</v>
       </c>
       <c r="CB4" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="CC4" s="2">
         <v>7</v>
       </c>
       <c r="CD4" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="CE4" s="2">
         <v>4</v>
@@ -2138,250 +2141,250 @@
     </row>
     <row r="5" spans="1:83">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>281</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2">
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I5" s="2">
         <v>10</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M5" s="2">
+        <v>7</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O5" s="2">
+        <v>8</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>9</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S5" s="2">
+        <v>8</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M5" s="2">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2" t="s">
+      <c r="U5" s="2">
+        <v>8</v>
+      </c>
+      <c r="V5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="O5" s="2">
-        <v>8</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="W5" s="2">
+        <v>7</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="Q5" s="2">
-        <v>9</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="S5" s="2">
-        <v>8</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="U5" s="2">
-        <v>8</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="W5" s="2">
-        <v>7</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="Y5" s="2">
         <v>7</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AA5" s="2">
         <v>3</v>
       </c>
       <c r="AB5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>7</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>8</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AO5" s="2">
+        <v>10</v>
+      </c>
+      <c r="AP5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AC5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>7</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
+      <c r="AQ5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AR5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AK5" s="2">
-        <v>8</v>
-      </c>
-      <c r="AL5" s="2" t="s">
+      <c r="AS5" s="2">
+        <v>8</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AM5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AN5" s="2" t="s">
+      <c r="AW5" s="2">
+        <v>9</v>
+      </c>
+      <c r="AX5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AO5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AP5" s="2" t="s">
+      <c r="AY5" s="2">
+        <v>8</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AQ5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AR5" s="2" t="s">
+      <c r="BA5" s="2">
+        <v>8</v>
+      </c>
+      <c r="BB5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AS5" s="2">
-        <v>8</v>
-      </c>
-      <c r="AT5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU5" s="2">
-        <v>7</v>
-      </c>
-      <c r="AV5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AW5" s="2">
-        <v>9</v>
-      </c>
-      <c r="AX5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AY5" s="2">
-        <v>8</v>
-      </c>
-      <c r="AZ5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BA5" s="2">
-        <v>8</v>
-      </c>
-      <c r="BB5" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="BC5" s="2">
         <v>8</v>
       </c>
       <c r="BD5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="BE5" s="2">
         <v>2</v>
       </c>
       <c r="BF5" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="BG5" s="2">
         <v>8</v>
       </c>
       <c r="BH5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI5" s="2">
         <v>3</v>
       </c>
       <c r="BJ5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="BK5" s="2">
         <v>5</v>
       </c>
       <c r="BL5" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="BM5" s="2">
         <v>6</v>
       </c>
       <c r="BN5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BO5" s="2">
         <v>4</v>
       </c>
       <c r="BP5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BQ5" s="2">
         <v>3</v>
       </c>
       <c r="BR5" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="BS5" s="2">
         <v>7</v>
       </c>
       <c r="BT5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="BU5" s="2">
         <v>6</v>
       </c>
       <c r="BV5" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="BW5" s="2">
         <v>4</v>
       </c>
       <c r="BX5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="BY5" s="2">
         <v>7</v>
       </c>
       <c r="BZ5" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="CA5" s="2">
         <v>1</v>
       </c>
       <c r="CB5" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="CC5" s="2">
         <v>7</v>
       </c>
       <c r="CD5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="CE5" s="2">
         <v>6</v>
@@ -2389,7 +2392,7 @@
     </row>
     <row r="6" spans="1:83">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>282</v>
       </c>
       <c r="B6" s="2">
         <v>1670</v>
@@ -2398,241 +2401,241 @@
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G6" s="2">
         <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I6" s="2">
         <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K6" s="2">
         <v>9</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="M6" s="2">
         <v>9</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="O6" s="2">
         <v>9</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="Q6" s="2">
         <v>10</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S6" s="2">
         <v>9</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="U6" s="2">
         <v>4</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="W6" s="2">
         <v>3</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="Y6" s="2">
         <v>3</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AA6" s="2">
         <v>8</v>
       </c>
       <c r="AB6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE6" s="2">
+        <v>7</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>8</v>
+      </c>
+      <c r="AJ6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>8</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AP6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AR6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>10</v>
+      </c>
+      <c r="AT6" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>9</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>7</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>9</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>8</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>8</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AO6" s="2">
-        <v>10</v>
-      </c>
-      <c r="AP6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AQ6" s="2">
-        <v>10</v>
-      </c>
-      <c r="AR6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS6" s="2">
-        <v>10</v>
-      </c>
-      <c r="AT6" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="AU6" s="2">
         <v>1</v>
       </c>
       <c r="AV6" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="AW6" s="2">
         <v>8</v>
       </c>
       <c r="AX6" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="AY6" s="2">
         <v>6</v>
       </c>
       <c r="AZ6" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="BA6" s="2">
         <v>8</v>
       </c>
       <c r="BB6" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="BC6" s="2">
         <v>5</v>
       </c>
       <c r="BD6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="BE6" s="2">
+        <v>9</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BG6" s="2">
+        <v>8</v>
+      </c>
+      <c r="BH6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BI6" s="2">
+        <v>9</v>
+      </c>
+      <c r="BJ6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="BK6" s="2">
+        <v>8</v>
+      </c>
+      <c r="BL6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BM6" s="2">
+        <v>7</v>
+      </c>
+      <c r="BN6" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="BE6" s="2">
-        <v>9</v>
-      </c>
-      <c r="BF6" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="BG6" s="2">
-        <v>8</v>
-      </c>
-      <c r="BH6" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="BI6" s="2">
-        <v>9</v>
-      </c>
-      <c r="BJ6" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="BK6" s="2">
-        <v>8</v>
-      </c>
-      <c r="BL6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="BM6" s="2">
-        <v>7</v>
-      </c>
-      <c r="BN6" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="BO6" s="2">
         <v>5</v>
       </c>
       <c r="BP6" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="BQ6" s="2">
         <v>10</v>
       </c>
       <c r="BR6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BS6" s="2">
+        <v>9</v>
+      </c>
+      <c r="BT6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="BS6" s="2">
-        <v>9</v>
-      </c>
-      <c r="BT6" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="BU6" s="2">
         <v>7</v>
       </c>
       <c r="BV6" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="BW6" s="2">
         <v>5</v>
       </c>
       <c r="BX6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="BY6" s="2">
         <v>8</v>
       </c>
       <c r="BZ6" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="CA6" s="2">
         <v>8</v>
       </c>
       <c r="CB6" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="CC6" s="2">
         <v>9</v>
       </c>
       <c r="CD6" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="CE6" s="2">
         <v>8</v>
@@ -2640,250 +2643,250 @@
     </row>
     <row r="7" spans="1:83">
       <c r="A7" s="2" t="s">
-        <v>158</v>
+        <v>283</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C7" s="2">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E7" s="2">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G7" s="2">
         <v>9</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I7" s="2">
         <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K7" s="2">
         <v>4</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="M7" s="2">
         <v>7</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="O7" s="2">
         <v>10</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="2">
         <v>6</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="S7" s="2">
         <v>9</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="U7" s="2">
         <v>5</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="W7" s="2">
         <v>9</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="Y7" s="2">
         <v>7</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="AA7" s="2">
         <v>8</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AC7" s="2">
         <v>7</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AE7" s="2">
         <v>10</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AG7" s="2">
         <v>9</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="AI7" s="2">
         <v>8</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AK7" s="2">
         <v>4</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AM7" s="2">
         <v>3</v>
       </c>
       <c r="AN7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO7" s="2">
         <v>2</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="AQ7" s="2">
         <v>5</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="AS7" s="2">
         <v>9</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AU7" s="2">
         <v>9</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="AW7" s="2">
         <v>10</v>
       </c>
       <c r="AX7" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="AY7" s="2">
         <v>2</v>
       </c>
       <c r="AZ7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="BA7" s="2">
         <v>7</v>
       </c>
       <c r="BB7" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="BC7" s="2">
         <v>8</v>
       </c>
       <c r="BD7" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="BE7" s="2">
         <v>8</v>
       </c>
       <c r="BF7" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="BG7" s="2">
         <v>9</v>
       </c>
       <c r="BH7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="BI7" s="2">
         <v>10</v>
       </c>
       <c r="BJ7" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="BK7" s="2">
         <v>6</v>
       </c>
       <c r="BL7" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="BM7" s="2">
         <v>1</v>
       </c>
       <c r="BN7" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BO7" s="2">
         <v>1</v>
       </c>
       <c r="BP7" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="BQ7" s="2">
         <v>2</v>
       </c>
       <c r="BR7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="BS7" s="2">
         <v>7</v>
       </c>
       <c r="BT7" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="BU7" s="2">
         <v>8</v>
       </c>
       <c r="BV7" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="BW7" s="2">
         <v>9</v>
       </c>
       <c r="BX7" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="BY7" s="2">
         <v>7</v>
       </c>
       <c r="BZ7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="CA7" s="2">
         <v>6</v>
       </c>
       <c r="CB7" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="CC7" s="2">
         <v>8</v>
       </c>
       <c r="CD7" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="CE7" s="2">
         <v>5</v>
@@ -2891,7 +2894,7 @@
     </row>
     <row r="8" spans="1:83">
       <c r="A8" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3">
         <v>1670</v>
@@ -2900,109 +2903,109 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2">
         <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2">
         <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2">
         <v>9</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K8" s="2">
         <v>10</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="M8" s="2">
         <v>9</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O8" s="2">
         <v>4</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="Q8" s="2">
         <v>6</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="S8" s="2">
         <v>6</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U8" s="2">
         <v>9</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="W8" s="2">
         <v>1</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="Y8" s="2">
         <v>7</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="AA8" s="2">
         <v>9</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AC8" s="2">
         <v>8</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="AE8" s="2">
         <v>7</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AG8" s="2">
         <v>3</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AI8" s="2">
         <v>3</v>
       </c>
       <c r="AJ8" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="AK8" s="2">
         <v>10</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AM8" s="2">
         <v>10</v>
@@ -3014,127 +3017,127 @@
         <v>10</v>
       </c>
       <c r="AP8" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="AQ8" s="2">
         <v>10</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AS8" s="2">
         <v>10</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="AU8" s="2">
         <v>10</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="AW8" s="2">
         <v>9</v>
       </c>
       <c r="AX8" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AY8" s="2">
         <v>2</v>
       </c>
       <c r="AZ8" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="BA8" s="2">
         <v>10</v>
       </c>
       <c r="BB8" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="BC8" s="2">
         <v>7</v>
       </c>
       <c r="BD8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="BE8" s="2">
         <v>8</v>
       </c>
       <c r="BF8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="BG8" s="2">
         <v>8</v>
       </c>
       <c r="BH8" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="BI8" s="2">
         <v>10</v>
       </c>
       <c r="BJ8" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="BK8" s="2">
         <v>10</v>
       </c>
       <c r="BL8" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BM8" s="2">
         <v>1</v>
       </c>
       <c r="BN8" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="BO8" s="2">
         <v>2</v>
       </c>
       <c r="BP8" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="BQ8" s="2">
         <v>2</v>
       </c>
       <c r="BR8" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="BS8" s="2">
         <v>2</v>
       </c>
       <c r="BT8" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="BU8" s="2">
         <v>1</v>
       </c>
       <c r="BV8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BW8" s="2">
         <v>2</v>
       </c>
       <c r="BX8" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="BY8" s="2">
         <v>3</v>
       </c>
       <c r="BZ8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="CA8" s="2">
         <v>3</v>
       </c>
       <c r="CB8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="CC8" s="2">
         <v>5</v>
       </c>
       <c r="CD8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CE8" s="2">
         <v>3</v>
@@ -3142,250 +3145,250 @@
     </row>
     <row r="9" spans="1:83">
       <c r="A9" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C9" s="2">
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E9" s="2">
         <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="I9" s="2">
         <v>9</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K9" s="2">
         <v>9</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M9" s="2">
         <v>8</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="O9" s="2">
         <v>5</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="Q9" s="2">
         <v>7</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="S9" s="2">
         <v>3</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="U9" s="2">
         <v>7</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="W9" s="2">
         <v>6</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y9" s="2">
         <v>7</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AA9" s="2">
         <v>10</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AC9" s="2">
         <v>9</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE9" s="2">
         <v>7</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="AG9" s="2">
         <v>7</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AI9" s="2">
         <v>6</v>
       </c>
       <c r="AJ9" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="AK9" s="2">
         <v>4</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AM9" s="2">
         <v>8</v>
       </c>
       <c r="AN9" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AO9" s="2">
         <v>9</v>
       </c>
       <c r="AP9" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AQ9" s="2">
         <v>6</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="AS9" s="2">
         <v>4</v>
       </c>
       <c r="AT9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AU9" s="2">
         <v>3</v>
       </c>
       <c r="AV9" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AW9" s="2">
         <v>8</v>
       </c>
       <c r="AX9" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="AY9" s="2">
         <v>5</v>
       </c>
       <c r="AZ9" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="BA9" s="2">
         <v>7</v>
       </c>
       <c r="BB9" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="BC9" s="2">
         <v>6</v>
       </c>
       <c r="BD9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="BE9" s="2">
         <v>5</v>
       </c>
       <c r="BF9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="BG9" s="2">
         <v>7</v>
       </c>
       <c r="BH9" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="BI9" s="2">
         <v>5</v>
       </c>
       <c r="BJ9" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="BK9" s="2">
         <v>6</v>
       </c>
       <c r="BL9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="BM9" s="2">
         <v>5</v>
       </c>
       <c r="BN9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="BO9" s="2">
         <v>2</v>
       </c>
       <c r="BP9" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="BQ9" s="2">
         <v>2</v>
       </c>
       <c r="BR9" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="BS9" s="2">
         <v>1</v>
       </c>
       <c r="BT9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="BU9" s="2">
         <v>7</v>
       </c>
       <c r="BV9" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="BW9" s="2">
         <v>3</v>
       </c>
       <c r="BX9" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="BY9" s="2">
         <v>8</v>
       </c>
       <c r="BZ9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="CA9" s="2">
         <v>8</v>
       </c>
       <c r="CB9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="CC9" s="2">
         <v>2</v>
       </c>
       <c r="CD9" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="CE9" s="2">
         <v>7</v>
@@ -3393,148 +3396,148 @@
     </row>
     <row r="10" spans="1:83">
       <c r="A10" s="2" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G10" s="2">
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I10" s="2">
         <v>7</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" s="2">
         <v>7</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="M10" s="2">
         <v>8</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O10" s="2">
         <v>9</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="Q10" s="2">
         <v>5</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="S10" s="2">
         <v>4</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="U10" s="2">
         <v>9</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="W10" s="2">
         <v>3</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y10" s="2">
         <v>8</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="AA10" s="2">
         <v>6</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AC10" s="2">
         <v>7</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="AE10" s="2">
         <v>8</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="AG10" s="2">
         <v>8</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AI10" s="2">
         <v>7</v>
       </c>
       <c r="AJ10" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="AK10" s="2">
         <v>8</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AM10" s="2">
         <v>8</v>
       </c>
       <c r="AN10" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AO10" s="2">
         <v>6</v>
       </c>
       <c r="AP10" s="2" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="AQ10" s="2">
         <v>5</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="AS10" s="2">
         <v>8</v>
       </c>
       <c r="AT10" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="AU10" s="2">
         <v>8</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AW10" s="2">
         <v>7</v>
@@ -3576,7 +3579,7 @@
     </row>
     <row r="11" spans="1:83">
       <c r="A11" s="2" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
       <c r="B11" s="6">
         <v>1670</v>
@@ -3585,241 +3588,241 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G11" s="2">
         <v>8</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="I11" s="2">
         <v>9</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K11" s="2">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M11" s="2">
         <v>8</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="O11" s="2">
         <v>9</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q11" s="2">
         <v>10</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S11" s="2">
         <v>5</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U11" s="2">
         <v>7</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="W11" s="2">
         <v>10</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="Y11" s="2">
         <v>8</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="AA11" s="2">
         <v>7</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AC11" s="2">
         <v>8</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="AE11" s="2">
         <v>9</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="AG11" s="2">
         <v>8</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AI11" s="2">
         <v>5</v>
       </c>
       <c r="AJ11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AK11" s="2">
         <v>8</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AM11" s="2">
         <v>8</v>
       </c>
       <c r="AN11" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="AO11" s="2">
         <v>5</v>
       </c>
       <c r="AP11" s="2" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="AQ11" s="2">
         <v>7</v>
       </c>
       <c r="AR11" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="AS11" s="2">
         <v>8</v>
       </c>
       <c r="AT11" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="AU11" s="2">
         <v>7</v>
       </c>
       <c r="AV11" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="AW11" s="2">
         <v>8</v>
       </c>
       <c r="AX11" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="AY11" s="2">
         <v>8</v>
       </c>
       <c r="AZ11" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="BA11" s="2">
         <v>6</v>
       </c>
       <c r="BB11" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="BC11" s="2">
         <v>9</v>
       </c>
       <c r="BD11" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="BE11" s="2">
         <v>8</v>
       </c>
       <c r="BF11" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="BG11" s="2">
         <v>8</v>
       </c>
       <c r="BH11" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="BI11" s="2">
         <v>7</v>
       </c>
       <c r="BJ11" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="BK11" s="2">
         <v>9</v>
       </c>
       <c r="BL11" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="BM11" s="2">
         <v>4</v>
       </c>
       <c r="BN11" s="2" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="BO11" s="2">
         <v>9</v>
       </c>
       <c r="BP11" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="BQ11" s="2">
         <v>6</v>
       </c>
       <c r="BR11" s="2" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="BS11" s="2">
         <v>6</v>
       </c>
       <c r="BT11" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="BU11" s="2">
         <v>10</v>
       </c>
       <c r="BV11" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="BW11" s="2">
         <v>10</v>
       </c>
       <c r="BX11" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="BY11" s="2">
         <v>9</v>
       </c>
       <c r="BZ11" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="CA11" s="2">
         <v>7</v>
       </c>
       <c r="CB11" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="CC11" s="2">
         <v>10</v>
       </c>
       <c r="CD11" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="CE11" s="2">
         <v>7</v>
@@ -3827,7 +3830,7 @@
     </row>
     <row r="12" spans="1:83">
       <c r="A12" s="2" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="B12" s="2">
         <v>1670</v>
@@ -3836,241 +3839,241 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E12" s="2">
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="G12" s="2">
         <v>8</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="I12" s="2">
         <v>7</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="K12" s="2">
         <v>8</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="M12" s="2">
         <v>7</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="O12" s="2">
         <v>6</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="Q12" s="2">
         <v>9</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="S12" s="2">
         <v>9</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="U12" s="2">
         <v>8</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="W12" s="2">
         <v>8</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="Y12" s="2">
         <v>9</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AA12" s="2">
         <v>1</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AC12" s="2">
         <v>8</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="AE12" s="2">
         <v>10</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="AG12" s="2">
         <v>8</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="AI12" s="2">
         <v>7</v>
       </c>
       <c r="AJ12" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="AK12" s="2">
         <v>8</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AM12" s="2">
         <v>9</v>
       </c>
       <c r="AN12" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="AO12" s="2">
         <v>6</v>
       </c>
       <c r="AP12" s="2" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="AQ12" s="2">
         <v>10</v>
       </c>
       <c r="AR12" s="2" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="AS12" s="2">
         <v>7</v>
       </c>
       <c r="AT12" s="2" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="AU12" s="2">
         <v>8</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="AW12" s="2">
         <v>7</v>
       </c>
       <c r="AX12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AY12" s="2">
         <v>6</v>
       </c>
       <c r="AZ12" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="BA12" s="2">
         <v>7</v>
       </c>
       <c r="BB12" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="BC12" s="2">
         <v>7</v>
       </c>
       <c r="BD12" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="BE12" s="2">
         <v>7</v>
       </c>
       <c r="BF12" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="BG12" s="2">
         <v>2</v>
       </c>
       <c r="BH12" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="BI12" s="2">
         <v>5</v>
       </c>
       <c r="BJ12" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="BK12" s="2">
         <v>5</v>
       </c>
       <c r="BL12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BM12" s="2">
         <v>8</v>
       </c>
       <c r="BN12" s="2" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="BO12" s="2">
         <v>7</v>
       </c>
       <c r="BP12" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="BQ12" s="2">
         <v>3</v>
       </c>
       <c r="BR12" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="BS12" s="2">
         <v>7</v>
       </c>
       <c r="BT12" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="BU12" s="2">
         <v>8</v>
       </c>
       <c r="BV12" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="BW12" s="2">
         <v>8</v>
       </c>
       <c r="BX12" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="BY12" s="2">
         <v>6</v>
       </c>
       <c r="BZ12" s="2" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="CA12" s="2">
         <v>3</v>
       </c>
       <c r="CB12" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="CC12" s="2">
         <v>7</v>
       </c>
       <c r="CD12" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="CE12" s="2">
         <v>9</v>

</xml_diff>